<commit_message>
2019-07-09 MRI project developing
</commit_message>
<xml_diff>
--- a/HH_Projects/01_Market_Risk_Indicator/Data_Files/Test_Files/measures_testing.xlsx
+++ b/HH_Projects/01_Market_Risk_Indicator/Data_Files/Test_Files/measures_testing.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\_Job\GitHub Repository\HH_Codebase\HH_Projects\01_Market_Risk_Indicator\Data_Files\Test_Files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{06D0C062-3266-4731-9CBC-6E904A5E2172}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2A774DCE-2608-4F40-8B3B-DA77EC154BD9}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{E3114BC9-20DC-4CE9-A218-AE988E57F90C}"/>
+    <workbookView xWindow="-23148" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{E3114BC9-20DC-4CE9-A218-AE988E57F90C}"/>
   </bookViews>
   <sheets>
     <sheet name="Full measures 2000-01-31" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="72">
   <si>
     <t xml:space="preserve">                   Factor  Next Returns</t>
   </si>
@@ -234,6 +234,18 @@
   </si>
   <si>
     <t>0.051404</t>
+  </si>
+  <si>
+    <t>Fmb_mcaps</t>
+  </si>
+  <si>
+    <t>1.263553</t>
+  </si>
+  <si>
+    <t>Fmb_mcaps_std</t>
+  </si>
+  <si>
+    <t>0.065432</t>
   </si>
 </sst>
 </file>
@@ -302,13 +314,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -320,6 +326,12 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -638,7 +650,7 @@
   <dimension ref="A1:R25"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="H1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="J16" sqref="J16"/>
+      <selection activeCell="K7" sqref="K7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -649,91 +661,91 @@
     <col min="8" max="11" width="19" customWidth="1"/>
     <col min="12" max="13" width="19" hidden="1" customWidth="1"/>
     <col min="14" max="14" width="19" customWidth="1"/>
-    <col min="16" max="16" width="12" customWidth="1"/>
+    <col min="16" max="16" width="16.109375" customWidth="1"/>
     <col min="17" max="18" width="14.44140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:18">
-      <c r="A1" s="3" t="s">
+      <c r="A1" s="9" t="s">
         <v>24</v>
       </c>
-      <c r="B1" s="3"/>
-      <c r="C1" s="3"/>
-      <c r="E1" s="3" t="s">
+      <c r="B1" s="9"/>
+      <c r="C1" s="9"/>
+      <c r="E1" s="9" t="s">
         <v>25</v>
       </c>
-      <c r="F1" s="3"/>
-      <c r="G1" s="4"/>
-      <c r="H1" s="6" t="s">
+      <c r="F1" s="9"/>
+      <c r="G1" s="3"/>
+      <c r="H1" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="I1" s="6"/>
-      <c r="J1" s="5"/>
-      <c r="K1" s="5"/>
-      <c r="L1" s="5"/>
-      <c r="M1" s="5"/>
-      <c r="N1" s="5"/>
-      <c r="O1" s="7"/>
-      <c r="P1" s="6" t="s">
+      <c r="I1" s="8"/>
+      <c r="J1" s="4"/>
+      <c r="K1" s="4"/>
+      <c r="L1" s="4"/>
+      <c r="M1" s="4"/>
+      <c r="N1" s="4"/>
+      <c r="O1" s="5"/>
+      <c r="P1" s="8" t="s">
         <v>29</v>
       </c>
-      <c r="Q1" s="6"/>
-      <c r="R1" s="6"/>
+      <c r="Q1" s="8"/>
+      <c r="R1" s="8"/>
     </row>
     <row r="2" spans="1:18">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="H2" s="6"/>
-      <c r="I2" s="6"/>
-      <c r="J2" s="5"/>
-      <c r="K2" s="5"/>
-      <c r="L2" s="5"/>
-      <c r="M2" s="5"/>
-      <c r="N2" s="5"/>
-      <c r="O2" s="7"/>
-      <c r="P2" s="6"/>
-      <c r="Q2" s="6"/>
-      <c r="R2" s="6"/>
+      <c r="H2" s="8"/>
+      <c r="I2" s="8"/>
+      <c r="J2" s="4"/>
+      <c r="K2" s="4"/>
+      <c r="L2" s="4"/>
+      <c r="M2" s="4"/>
+      <c r="N2" s="4"/>
+      <c r="O2" s="5"/>
+      <c r="P2" s="8"/>
+      <c r="Q2" s="8"/>
+      <c r="R2" s="8"/>
     </row>
     <row r="3" spans="1:18" ht="36" customHeight="1">
       <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="E3" s="5" t="s">
+      <c r="E3" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="F3" s="5" t="s">
+      <c r="F3" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="G3" s="5"/>
-      <c r="H3" s="9" t="s">
+      <c r="G3" s="4"/>
+      <c r="H3" s="7" t="s">
         <v>41</v>
       </c>
-      <c r="I3" s="9" t="s">
+      <c r="I3" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="J3" s="9" t="s">
+      <c r="J3" s="7" t="s">
         <v>37</v>
       </c>
-      <c r="K3" s="9" t="s">
+      <c r="K3" s="7" t="s">
         <v>38</v>
       </c>
-      <c r="L3" s="9" t="s">
+      <c r="L3" s="7" t="s">
         <v>65</v>
       </c>
-      <c r="M3" s="9"/>
-      <c r="N3" s="9" t="s">
+      <c r="M3" s="7"/>
+      <c r="N3" s="7" t="s">
         <v>66</v>
       </c>
       <c r="O3" s="2"/>
-      <c r="P3" s="9" t="s">
+      <c r="P3" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="Q3" s="9" t="s">
+      <c r="Q3" s="7" t="s">
         <v>30</v>
       </c>
-      <c r="R3" s="9" t="s">
+      <c r="R3" s="7" t="s">
         <v>31</v>
       </c>
     </row>
@@ -773,7 +785,7 @@
       <c r="N4">
         <v>-0.44741199999999998</v>
       </c>
-      <c r="P4" s="8" t="s">
+      <c r="P4" s="6" t="s">
         <v>33</v>
       </c>
       <c r="Q4">
@@ -820,7 +832,7 @@
       <c r="N5">
         <v>0.62212400000000001</v>
       </c>
-      <c r="P5" s="8" t="s">
+      <c r="P5" s="6" t="s">
         <v>35</v>
       </c>
       <c r="Q5">
@@ -867,7 +879,7 @@
       <c r="N6">
         <v>-2.021566</v>
       </c>
-      <c r="P6" s="8" t="s">
+      <c r="P6" s="6" t="s">
         <v>39</v>
       </c>
       <c r="Q6">
@@ -914,7 +926,7 @@
       <c r="N7">
         <v>1.4307799999999999</v>
       </c>
-      <c r="P7" s="8" t="s">
+      <c r="P7" s="6" t="s">
         <v>42</v>
       </c>
       <c r="Q7">
@@ -961,7 +973,12 @@
       <c r="N8">
         <v>-0.90624099999999996</v>
       </c>
-      <c r="P8" s="8"/>
+      <c r="P8" s="6" t="s">
+        <v>68</v>
+      </c>
+      <c r="R8" t="s">
+        <v>69</v>
+      </c>
     </row>
     <row r="9" spans="1:18">
       <c r="A9" s="1" t="s">
@@ -999,7 +1016,12 @@
       <c r="N9">
         <v>0.64790800000000004</v>
       </c>
-      <c r="P9" s="8"/>
+      <c r="P9" s="6" t="s">
+        <v>70</v>
+      </c>
+      <c r="R9" t="s">
+        <v>71</v>
+      </c>
     </row>
     <row r="10" spans="1:18">
       <c r="A10" s="1" t="s">
@@ -1037,7 +1059,7 @@
       <c r="N10">
         <v>0.253668</v>
       </c>
-      <c r="P10" s="8"/>
+      <c r="P10" s="6"/>
     </row>
     <row r="11" spans="1:18">
       <c r="A11" s="1" t="s">
@@ -1075,7 +1097,7 @@
       <c r="N11">
         <v>-0.24048800000000001</v>
       </c>
-      <c r="P11" s="8"/>
+      <c r="P11" s="6"/>
     </row>
     <row r="12" spans="1:18">
       <c r="A12" s="1" t="s">
@@ -1113,7 +1135,7 @@
       <c r="N12">
         <v>1.3818349999999999</v>
       </c>
-      <c r="P12" s="8"/>
+      <c r="P12" s="6"/>
     </row>
     <row r="13" spans="1:18">
       <c r="A13" s="1" t="s">
@@ -1151,7 +1173,7 @@
       <c r="N13">
         <v>-1.554E-3</v>
       </c>
-      <c r="P13" s="8"/>
+      <c r="P13" s="6"/>
     </row>
     <row r="14" spans="1:18">
       <c r="A14" s="1" t="s">
@@ -1189,7 +1211,7 @@
       <c r="N14">
         <v>-0.52763599999999999</v>
       </c>
-      <c r="P14" s="8"/>
+      <c r="P14" s="6"/>
     </row>
     <row r="15" spans="1:18">
       <c r="A15" s="1" t="s">

</xml_diff>

<commit_message>
2019-07-12 MRI project developing
</commit_message>
<xml_diff>
--- a/HH_Projects/01_Market_Risk_Indicator/Data_Files/Test_Files/measures_testing.xlsx
+++ b/HH_Projects/01_Market_Risk_Indicator/Data_Files/Test_Files/measures_testing.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\_Job\GitHub Repository\HH_Codebase\HH_Projects\01_Market_Risk_Indicator\Data_Files\Test_Files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2A774DCE-2608-4F40-8B3B-DA77EC154BD9}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{447E72FA-E6A4-4E16-9D8F-88A3C849BAA8}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-23148" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{E3114BC9-20DC-4CE9-A218-AE988E57F90C}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{E3114BC9-20DC-4CE9-A218-AE988E57F90C}"/>
   </bookViews>
   <sheets>
     <sheet name="Full measures 2000-01-31" sheetId="1" r:id="rId1"/>
@@ -650,7 +650,7 @@
   <dimension ref="A1:R25"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="H1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="K7" sqref="K7"/>
+      <selection activeCell="K13" sqref="K13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -786,14 +786,14 @@
         <v>-0.44741199999999998</v>
       </c>
       <c r="P4" s="6" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="Q4">
-        <f>PEARSON(H4:H25,I4:I25)</f>
-        <v>0.6189873708392758</v>
+        <f>CORREL(J4:J25,K4:K25)</f>
+        <v>0.63975155279503104</v>
       </c>
       <c r="R4" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
     </row>
     <row r="5" spans="1:18">
@@ -833,14 +833,14 @@
         <v>0.62212400000000001</v>
       </c>
       <c r="P5" s="6" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="Q5">
-        <f>CORREL(J4:J25,K4:K25)</f>
-        <v>0.63975155279503104</v>
+        <f>PEARSON(H4:H25,I4:I25)</f>
+        <v>0.6189873708392758</v>
       </c>
       <c r="R5" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
     </row>
     <row r="6" spans="1:18">
@@ -1097,7 +1097,6 @@
       <c r="N11">
         <v>-0.24048800000000001</v>
       </c>
-      <c r="P11" s="6"/>
     </row>
     <row r="12" spans="1:18">
       <c r="A12" s="1" t="s">

</xml_diff>